<commit_message>
grad + ativ comunitarias
</commit_message>
<xml_diff>
--- a/dados_graduacao/Tabela2.10.xlsx
+++ b/dados_graduacao/Tabela2.10.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="370">
   <si>
     <t xml:space="preserve">Unidade acadêmica / curso / habilitação</t>
   </si>
@@ -371,7 +371,10 @@
     <t xml:space="preserve">Educação Física (L - A Distância)</t>
   </si>
   <si>
-    <t xml:space="preserve">NA%</t>
+    <t xml:space="preserve">100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
   </si>
   <si>
     <t xml:space="preserve">Educação Física (L - Integral)</t>
@@ -722,9 +725,6 @@
     <t xml:space="preserve">94.3%</t>
   </si>
   <si>
-    <t xml:space="preserve">Educação Artística-Música (L - Integral)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Música-Canto (B - Integral)</t>
   </si>
   <si>
@@ -765,9 +765,6 @@
   </si>
   <si>
     <t xml:space="preserve">77.7%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teatro (L - A Distância)</t>
   </si>
   <si>
     <t xml:space="preserve">Teoria Crítica e História da Arte (B - Noturno)</t>
@@ -2681,25 +2678,31 @@
       <c r="B43" t="n">
         <v>6</v>
       </c>
-      <c r="C43"/>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
       <c r="D43" t="n">
         <v>4</v>
       </c>
-      <c r="E43"/>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
       <c r="F43" t="n">
         <v>4</v>
       </c>
-      <c r="G43"/>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
       <c r="H43" t="s">
         <v>119</v>
       </c>
       <c r="I43" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B44" t="n">
         <v>346</v>
@@ -2728,7 +2731,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B45" t="n">
         <v>2164</v>
@@ -2749,15 +2752,15 @@
         <v>8124</v>
       </c>
       <c r="H45" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I45" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B46" t="n">
         <v>530</v>
@@ -2778,15 +2781,15 @@
         <v>1689</v>
       </c>
       <c r="H46" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I46" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B47" t="n">
         <v>315</v>
@@ -2807,15 +2810,15 @@
         <v>1223</v>
       </c>
       <c r="H47" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I47" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B48" t="n">
         <v>165</v>
@@ -2836,15 +2839,15 @@
         <v>623</v>
       </c>
       <c r="H48" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I48" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B49" t="n">
         <v>231</v>
@@ -2865,15 +2868,15 @@
         <v>883</v>
       </c>
       <c r="H49" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I49" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B50" t="n">
         <v>541</v>
@@ -2894,15 +2897,15 @@
         <v>2297</v>
       </c>
       <c r="H50" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I50" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B51" t="n">
         <v>382</v>
@@ -2923,15 +2926,15 @@
         <v>1409</v>
       </c>
       <c r="H51" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I51" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B52" t="n">
         <v>527</v>
@@ -2952,15 +2955,15 @@
         <v>2789</v>
       </c>
       <c r="H52" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I52" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B53" t="n">
         <v>527</v>
@@ -2981,15 +2984,15 @@
         <v>2789</v>
       </c>
       <c r="H53" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I53" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B54" t="n">
         <v>1725</v>
@@ -3013,12 +3016,12 @@
         <v>47</v>
       </c>
       <c r="I54" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B55" t="n">
         <v>342</v>
@@ -3047,7 +3050,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B56" t="n">
         <v>218</v>
@@ -3068,15 +3071,15 @@
         <v>928</v>
       </c>
       <c r="H56" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I56" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B57" t="n">
         <v>374</v>
@@ -3097,7 +3100,7 @@
         <v>1620</v>
       </c>
       <c r="H57" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I57" t="s">
         <v>51</v>
@@ -3105,7 +3108,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B58" t="n">
         <v>243</v>
@@ -3134,7 +3137,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B59" t="n">
         <v>281</v>
@@ -3155,7 +3158,7 @@
         <v>1348</v>
       </c>
       <c r="H59" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I59" t="s">
         <v>18</v>
@@ -3163,7 +3166,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B60" t="n">
         <v>267</v>
@@ -3184,15 +3187,15 @@
         <v>1335</v>
       </c>
       <c r="H60" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I60" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B61" t="n">
         <v>3100</v>
@@ -3216,12 +3219,12 @@
         <v>56</v>
       </c>
       <c r="I61" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B62" t="n">
         <v>332</v>
@@ -3245,12 +3248,12 @@
         <v>56</v>
       </c>
       <c r="I62" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B63" t="n">
         <v>402</v>
@@ -3274,12 +3277,12 @@
         <v>91</v>
       </c>
       <c r="I63" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B64" t="n">
         <v>524</v>
@@ -3303,12 +3306,12 @@
         <v>20</v>
       </c>
       <c r="I64" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B65" t="n">
         <v>287</v>
@@ -3329,15 +3332,15 @@
         <v>1158</v>
       </c>
       <c r="H65" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I65" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B66" t="n">
         <v>403</v>
@@ -3358,15 +3361,15 @@
         <v>1762</v>
       </c>
       <c r="H66" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I66" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B67" t="n">
         <v>388</v>
@@ -3390,12 +3393,12 @@
         <v>41</v>
       </c>
       <c r="I67" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B68" t="n">
         <v>404</v>
@@ -3416,15 +3419,15 @@
         <v>1671</v>
       </c>
       <c r="H68" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I68" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B69" t="n">
         <v>360</v>
@@ -3445,15 +3448,15 @@
         <v>1533</v>
       </c>
       <c r="H69" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I69" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B70" t="n">
         <v>1013</v>
@@ -3474,15 +3477,15 @@
         <v>4445</v>
       </c>
       <c r="H70" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I70" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B71" t="n">
         <v>172</v>
@@ -3503,7 +3506,7 @@
         <v>682</v>
       </c>
       <c r="H71" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I71" t="s">
         <v>27</v>
@@ -3511,7 +3514,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B72" t="n">
         <v>153</v>
@@ -3532,15 +3535,15 @@
         <v>586</v>
       </c>
       <c r="H72" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I72" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B73" t="n">
         <v>246</v>
@@ -3561,15 +3564,15 @@
         <v>1705</v>
       </c>
       <c r="H73" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I73" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B74" t="n">
         <v>226</v>
@@ -3590,15 +3593,15 @@
         <v>729</v>
       </c>
       <c r="H74" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I74" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B75" t="n">
         <v>216</v>
@@ -3619,15 +3622,15 @@
         <v>743</v>
       </c>
       <c r="H75" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I75" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B76" t="n">
         <v>990</v>
@@ -3648,7 +3651,7 @@
         <v>4692</v>
       </c>
       <c r="H76" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="I76" t="s">
         <v>74</v>
@@ -3656,7 +3659,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B77" t="n">
         <v>262</v>
@@ -3680,12 +3683,12 @@
         <v>92</v>
       </c>
       <c r="I77" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B78" t="n">
         <v>344</v>
@@ -3714,7 +3717,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B79" t="n">
         <v>9</v>
@@ -3735,7 +3738,7 @@
         <v>7</v>
       </c>
       <c r="H79" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I79" t="s">
         <v>119</v>
@@ -3743,7 +3746,7 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B80" t="n">
         <v>375</v>
@@ -3764,15 +3767,15 @@
         <v>1620</v>
       </c>
       <c r="H80" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I80" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B81" t="n">
         <v>727</v>
@@ -3793,7 +3796,7 @@
         <v>2284</v>
       </c>
       <c r="H81" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I81" t="s">
         <v>98</v>
@@ -3801,7 +3804,7 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B82" t="n">
         <v>84</v>
@@ -3825,12 +3828,12 @@
         <v>35</v>
       </c>
       <c r="I82" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B83" t="n">
         <v>144</v>
@@ -3851,15 +3854,15 @@
         <v>554</v>
       </c>
       <c r="H83" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I83" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B84" t="n">
         <v>81</v>
@@ -3880,15 +3883,15 @@
         <v>207</v>
       </c>
       <c r="H84" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I84" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B85" t="n">
         <v>163</v>
@@ -3909,7 +3912,7 @@
         <v>570</v>
       </c>
       <c r="H85" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I85" t="s">
         <v>54</v>
@@ -3917,7 +3920,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B86" t="n">
         <v>255</v>
@@ -3941,12 +3944,12 @@
         <v>26</v>
       </c>
       <c r="I86" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B87" t="n">
         <v>1458</v>
@@ -3970,12 +3973,12 @@
         <v>54</v>
       </c>
       <c r="I87" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B88" t="n">
         <v>50</v>
@@ -4004,7 +4007,7 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B89" t="n">
         <v>91</v>
@@ -4033,7 +4036,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B90" t="n">
         <v>84</v>
@@ -4057,12 +4060,12 @@
         <v>27</v>
       </c>
       <c r="I90" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B91" t="n">
         <v>71</v>
@@ -4091,7 +4094,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B92" t="n">
         <v>60</v>
@@ -4115,12 +4118,12 @@
         <v>66</v>
       </c>
       <c r="I92" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B93" t="n">
         <v>115</v>
@@ -4141,15 +4144,15 @@
         <v>293</v>
       </c>
       <c r="H93" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I93" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B94" t="n">
         <v>110</v>
@@ -4170,15 +4173,15 @@
         <v>364</v>
       </c>
       <c r="H94" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="I94" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B95" t="n">
         <v>100</v>
@@ -4199,38 +4202,44 @@
         <v>329</v>
       </c>
       <c r="H95" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I95" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B96" t="n">
         <v>2</v>
       </c>
-      <c r="C96"/>
+      <c r="C96" t="n">
+        <v>0</v>
+      </c>
       <c r="D96" t="n">
         <v>7</v>
       </c>
-      <c r="E96"/>
+      <c r="E96" t="n">
+        <v>0</v>
+      </c>
       <c r="F96" t="n">
         <v>7</v>
       </c>
-      <c r="G96"/>
+      <c r="G96" t="n">
+        <v>0</v>
+      </c>
       <c r="H96" t="s">
         <v>119</v>
       </c>
       <c r="I96" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B97" t="n">
         <v>129</v>
@@ -4254,12 +4263,12 @@
         <v>66</v>
       </c>
       <c r="I97" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B98" t="n">
         <v>48</v>
@@ -4280,15 +4289,15 @@
         <v>116</v>
       </c>
       <c r="H98" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I98" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B99" t="n">
         <v>38</v>
@@ -4312,2261 +4321,2239 @@
         <v>80</v>
       </c>
       <c r="I99" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>236</v>
-      </c>
-      <c r="B100"/>
-      <c r="C100"/>
-      <c r="D100"/>
-      <c r="E100"/>
-      <c r="F100"/>
-      <c r="G100"/>
+        <v>237</v>
+      </c>
+      <c r="B100" t="n">
+        <v>46</v>
+      </c>
+      <c r="C100" t="n">
+        <v>35</v>
+      </c>
+      <c r="D100" t="n">
+        <v>176</v>
+      </c>
+      <c r="E100" t="n">
+        <v>149</v>
+      </c>
+      <c r="F100" t="n">
+        <v>157</v>
+      </c>
+      <c r="G100" t="n">
+        <v>135</v>
+      </c>
       <c r="H100" t="s">
-        <v>119</v>
+        <v>233</v>
       </c>
       <c r="I100" t="s">
-        <v>119</v>
+        <v>154</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B101" t="n">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C101" t="n">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D101" t="n">
-        <v>176</v>
+        <v>99</v>
       </c>
       <c r="E101" t="n">
-        <v>149</v>
+        <v>97</v>
       </c>
       <c r="F101" t="n">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="G101" t="n">
-        <v>135</v>
+        <v>79</v>
       </c>
       <c r="H101" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="I101" t="s">
-        <v>153</v>
+        <v>240</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B102" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C102" t="n">
+        <v>5</v>
+      </c>
+      <c r="D102" t="n">
+        <v>7</v>
+      </c>
+      <c r="E102" t="n">
+        <v>29</v>
+      </c>
+      <c r="F102" t="n">
+        <v>7</v>
+      </c>
+      <c r="G102" t="n">
         <v>26</v>
       </c>
-      <c r="D102" t="n">
-        <v>99</v>
-      </c>
-      <c r="E102" t="n">
-        <v>97</v>
-      </c>
-      <c r="F102" t="n">
-        <v>82</v>
-      </c>
-      <c r="G102" t="n">
-        <v>79</v>
-      </c>
       <c r="H102" t="s">
-        <v>239</v>
+        <v>119</v>
       </c>
       <c r="I102" t="s">
-        <v>240</v>
+        <v>50</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B103" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C103" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D103" t="n">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="E103" t="n">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="F103" t="n">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="G103" t="n">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="H103" t="s">
-        <v>119</v>
+        <v>243</v>
       </c>
       <c r="I103" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B104" t="n">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="C104" t="n">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D104" t="n">
-        <v>81</v>
+        <v>176</v>
       </c>
       <c r="E104" t="n">
-        <v>49</v>
+        <v>149</v>
       </c>
       <c r="F104" t="n">
-        <v>79</v>
+        <v>157</v>
       </c>
       <c r="G104" t="n">
-        <v>42</v>
+        <v>135</v>
       </c>
       <c r="H104" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="I104" t="s">
-        <v>23</v>
+        <v>154</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B105" t="n">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="C105" t="n">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="D105" t="n">
-        <v>176</v>
+        <v>17</v>
       </c>
       <c r="E105" t="n">
-        <v>149</v>
+        <v>6</v>
       </c>
       <c r="F105" t="n">
-        <v>157</v>
+        <v>15</v>
       </c>
       <c r="G105" t="n">
-        <v>135</v>
+        <v>4</v>
       </c>
       <c r="H105" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="I105" t="s">
-        <v>153</v>
+        <v>247</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B106" t="n">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="C106" t="n">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="D106" t="n">
-        <v>17</v>
+        <v>609</v>
       </c>
       <c r="E106" t="n">
-        <v>6</v>
+        <v>591</v>
       </c>
       <c r="F106" t="n">
-        <v>15</v>
+        <v>528</v>
       </c>
       <c r="G106" t="n">
-        <v>4</v>
+        <v>512</v>
       </c>
       <c r="H106" t="s">
-        <v>246</v>
+        <v>194</v>
       </c>
       <c r="I106" t="s">
-        <v>247</v>
+        <v>196</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B107" t="n">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="C107" t="n">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="D107" t="n">
-        <v>609</v>
+        <v>364</v>
       </c>
       <c r="E107" t="n">
-        <v>591</v>
+        <v>283</v>
       </c>
       <c r="F107" t="n">
-        <v>528</v>
+        <v>283</v>
       </c>
       <c r="G107" t="n">
-        <v>512</v>
+        <v>237</v>
       </c>
       <c r="H107" t="s">
-        <v>193</v>
+        <v>250</v>
       </c>
       <c r="I107" t="s">
-        <v>195</v>
+        <v>89</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B108" t="n">
-        <v>74</v>
+        <v>240</v>
       </c>
       <c r="C108" t="n">
-        <v>61</v>
+        <v>235</v>
       </c>
       <c r="D108" t="n">
-        <v>364</v>
+        <v>911</v>
       </c>
       <c r="E108" t="n">
-        <v>283</v>
+        <v>860</v>
       </c>
       <c r="F108" t="n">
-        <v>283</v>
+        <v>737</v>
       </c>
       <c r="G108" t="n">
-        <v>237</v>
+        <v>725</v>
       </c>
       <c r="H108" t="s">
-        <v>250</v>
+        <v>43</v>
       </c>
       <c r="I108" t="s">
-        <v>89</v>
+        <v>252</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>251</v>
-      </c>
-      <c r="B109"/>
-      <c r="C109"/>
-      <c r="D109"/>
-      <c r="E109"/>
-      <c r="F109"/>
-      <c r="G109"/>
+        <v>253</v>
+      </c>
+      <c r="B109" t="n">
+        <v>1602</v>
+      </c>
+      <c r="C109" t="n">
+        <v>1596</v>
+      </c>
+      <c r="D109" t="n">
+        <v>7684</v>
+      </c>
+      <c r="E109" t="n">
+        <v>7318</v>
+      </c>
+      <c r="F109" t="n">
+        <v>5758</v>
+      </c>
+      <c r="G109" t="n">
+        <v>5405</v>
+      </c>
       <c r="H109" t="s">
-        <v>119</v>
+        <v>254</v>
       </c>
       <c r="I109" t="s">
-        <v>119</v>
+        <v>185</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B110" t="n">
-        <v>240</v>
+        <v>346</v>
       </c>
       <c r="C110" t="n">
-        <v>235</v>
+        <v>345</v>
       </c>
       <c r="D110" t="n">
-        <v>911</v>
+        <v>1731</v>
       </c>
       <c r="E110" t="n">
-        <v>860</v>
+        <v>1601</v>
       </c>
       <c r="F110" t="n">
-        <v>737</v>
+        <v>1313</v>
       </c>
       <c r="G110" t="n">
-        <v>725</v>
+        <v>1254</v>
       </c>
       <c r="H110" t="s">
-        <v>43</v>
+        <v>256</v>
       </c>
       <c r="I110" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B111" t="n">
-        <v>1602</v>
+        <v>270</v>
       </c>
       <c r="C111" t="n">
-        <v>1596</v>
+        <v>271</v>
       </c>
       <c r="D111" t="n">
-        <v>7684</v>
+        <v>1127</v>
       </c>
       <c r="E111" t="n">
-        <v>7318</v>
+        <v>1083</v>
       </c>
       <c r="F111" t="n">
-        <v>5758</v>
+        <v>756</v>
       </c>
       <c r="G111" t="n">
-        <v>5405</v>
+        <v>762</v>
       </c>
       <c r="H111" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="I111" t="s">
-        <v>184</v>
+        <v>260</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="B112" t="n">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C112" t="n">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="D112" t="n">
-        <v>1731</v>
+        <v>1849</v>
       </c>
       <c r="E112" t="n">
-        <v>1601</v>
+        <v>1708</v>
       </c>
       <c r="F112" t="n">
-        <v>1313</v>
+        <v>1466</v>
       </c>
       <c r="G112" t="n">
-        <v>1254</v>
+        <v>1300</v>
       </c>
       <c r="H112" t="s">
-        <v>257</v>
+        <v>151</v>
       </c>
       <c r="I112" t="s">
-        <v>258</v>
+        <v>173</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B113" t="n">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C113" t="n">
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="D113" t="n">
-        <v>1127</v>
+        <v>1314</v>
       </c>
       <c r="E113" t="n">
-        <v>1083</v>
+        <v>1320</v>
       </c>
       <c r="F113" t="n">
-        <v>756</v>
+        <v>1057</v>
       </c>
       <c r="G113" t="n">
-        <v>762</v>
+        <v>981</v>
       </c>
       <c r="H113" t="s">
-        <v>260</v>
+        <v>176</v>
       </c>
       <c r="I113" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B114" t="n">
-        <v>344</v>
+        <v>58</v>
       </c>
       <c r="C114" t="n">
-        <v>321</v>
+        <v>61</v>
       </c>
       <c r="D114" t="n">
-        <v>1849</v>
+        <v>267</v>
       </c>
       <c r="E114" t="n">
-        <v>1708</v>
+        <v>286</v>
       </c>
       <c r="F114" t="n">
-        <v>1466</v>
+        <v>162</v>
       </c>
       <c r="G114" t="n">
-        <v>1300</v>
+        <v>165</v>
       </c>
       <c r="H114" t="s">
-        <v>150</v>
+        <v>265</v>
       </c>
       <c r="I114" t="s">
-        <v>172</v>
+        <v>266</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B115" t="n">
-        <v>269</v>
+        <v>36</v>
       </c>
       <c r="C115" t="n">
-        <v>284</v>
+        <v>31</v>
       </c>
       <c r="D115" t="n">
-        <v>1314</v>
+        <v>130</v>
       </c>
       <c r="E115" t="n">
-        <v>1320</v>
+        <v>101</v>
       </c>
       <c r="F115" t="n">
-        <v>1057</v>
+        <v>93</v>
       </c>
       <c r="G115" t="n">
-        <v>981</v>
+        <v>85</v>
       </c>
       <c r="H115" t="s">
-        <v>175</v>
+        <v>135</v>
       </c>
       <c r="I115" t="s">
-        <v>264</v>
+        <v>11</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B116" t="n">
-        <v>58</v>
+        <v>122</v>
       </c>
       <c r="C116" t="n">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="D116" t="n">
-        <v>267</v>
+        <v>576</v>
       </c>
       <c r="E116" t="n">
-        <v>286</v>
+        <v>546</v>
       </c>
       <c r="F116" t="n">
-        <v>162</v>
+        <v>434</v>
       </c>
       <c r="G116" t="n">
-        <v>165</v>
+        <v>389</v>
       </c>
       <c r="H116" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="I116" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B117" t="n">
-        <v>36</v>
+        <v>157</v>
       </c>
       <c r="C117" t="n">
-        <v>31</v>
+        <v>163</v>
       </c>
       <c r="D117" t="n">
-        <v>130</v>
+        <v>690</v>
       </c>
       <c r="E117" t="n">
-        <v>101</v>
+        <v>673</v>
       </c>
       <c r="F117" t="n">
-        <v>93</v>
+        <v>477</v>
       </c>
       <c r="G117" t="n">
-        <v>85</v>
+        <v>469</v>
       </c>
       <c r="H117" t="s">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="I117" t="s">
-        <v>11</v>
+        <v>272</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B118" t="n">
-        <v>122</v>
+        <v>371</v>
       </c>
       <c r="C118" t="n">
-        <v>120</v>
+        <v>350</v>
       </c>
       <c r="D118" t="n">
-        <v>576</v>
+        <v>1707</v>
       </c>
       <c r="E118" t="n">
-        <v>546</v>
+        <v>1538</v>
       </c>
       <c r="F118" t="n">
-        <v>434</v>
+        <v>1233</v>
       </c>
       <c r="G118" t="n">
-        <v>389</v>
+        <v>1150</v>
       </c>
       <c r="H118" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="I118" t="s">
-        <v>271</v>
+        <v>130</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B119" t="n">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="C119" t="n">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="D119" t="n">
-        <v>690</v>
+        <v>792</v>
       </c>
       <c r="E119" t="n">
-        <v>673</v>
+        <v>732</v>
       </c>
       <c r="F119" t="n">
-        <v>477</v>
+        <v>560</v>
       </c>
       <c r="G119" t="n">
-        <v>469</v>
+        <v>550</v>
       </c>
       <c r="H119" t="s">
-        <v>62</v>
+        <v>169</v>
       </c>
       <c r="I119" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B120" t="n">
-        <v>371</v>
+        <v>2</v>
       </c>
       <c r="C120" t="n">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="D120" t="n">
-        <v>1707</v>
+        <v>6</v>
       </c>
       <c r="E120" t="n">
-        <v>1538</v>
+        <v>0</v>
       </c>
       <c r="F120" t="n">
-        <v>1233</v>
+        <v>4</v>
       </c>
       <c r="G120" t="n">
-        <v>1150</v>
+        <v>0</v>
       </c>
       <c r="H120" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
       <c r="I120" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B121" t="n">
-        <v>173</v>
+        <v>195</v>
       </c>
       <c r="C121" t="n">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="D121" t="n">
-        <v>792</v>
+        <v>901</v>
       </c>
       <c r="E121" t="n">
-        <v>732</v>
+        <v>806</v>
       </c>
       <c r="F121" t="n">
-        <v>560</v>
+        <v>665</v>
       </c>
       <c r="G121" t="n">
-        <v>550</v>
+        <v>600</v>
       </c>
       <c r="H121" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="I121" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B122" t="n">
-        <v>2</v>
-      </c>
-      <c r="C122"/>
+        <v>1</v>
+      </c>
+      <c r="C122" t="n">
+        <v>0</v>
+      </c>
       <c r="D122" t="n">
-        <v>6</v>
-      </c>
-      <c r="E122"/>
+        <v>8</v>
+      </c>
+      <c r="E122" t="n">
+        <v>0</v>
+      </c>
       <c r="F122" t="n">
         <v>4</v>
       </c>
-      <c r="G122"/>
+      <c r="G122" t="n">
+        <v>0</v>
+      </c>
       <c r="H122" t="s">
-        <v>247</v>
+        <v>282</v>
       </c>
       <c r="I122" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B123" t="n">
-        <v>195</v>
+        <v>669</v>
       </c>
       <c r="C123" t="n">
-        <v>179</v>
+        <v>686</v>
       </c>
       <c r="D123" t="n">
-        <v>901</v>
+        <v>3326</v>
       </c>
       <c r="E123" t="n">
-        <v>806</v>
+        <v>3082</v>
       </c>
       <c r="F123" t="n">
-        <v>665</v>
+        <v>2575</v>
       </c>
       <c r="G123" t="n">
-        <v>600</v>
+        <v>2277</v>
       </c>
       <c r="H123" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="I123" t="s">
-        <v>281</v>
+        <v>185</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B124" t="n">
-        <v>1</v>
-      </c>
-      <c r="C124"/>
+        <v>280</v>
+      </c>
+      <c r="C124" t="n">
+        <v>289</v>
+      </c>
       <c r="D124" t="n">
-        <v>8</v>
-      </c>
-      <c r="E124"/>
+        <v>1305</v>
+      </c>
+      <c r="E124" t="n">
+        <v>1263</v>
+      </c>
       <c r="F124" t="n">
-        <v>4</v>
-      </c>
-      <c r="G124"/>
+        <v>1024</v>
+      </c>
+      <c r="G124" t="n">
+        <v>991</v>
+      </c>
       <c r="H124" t="s">
-        <v>283</v>
+        <v>59</v>
       </c>
       <c r="I124" t="s">
-        <v>119</v>
+        <v>59</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B125" t="n">
-        <v>669</v>
+        <v>136</v>
       </c>
       <c r="C125" t="n">
-        <v>686</v>
+        <v>134</v>
       </c>
       <c r="D125" t="n">
-        <v>3326</v>
+        <v>694</v>
       </c>
       <c r="E125" t="n">
-        <v>3082</v>
+        <v>627</v>
       </c>
       <c r="F125" t="n">
-        <v>2575</v>
+        <v>484</v>
       </c>
       <c r="G125" t="n">
-        <v>2277</v>
+        <v>374</v>
       </c>
       <c r="H125" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="I125" t="s">
-        <v>184</v>
+        <v>287</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B126" t="n">
-        <v>280</v>
+        <v>253</v>
       </c>
       <c r="C126" t="n">
+        <v>263</v>
+      </c>
+      <c r="D126" t="n">
+        <v>1327</v>
+      </c>
+      <c r="E126" t="n">
+        <v>1192</v>
+      </c>
+      <c r="F126" t="n">
+        <v>1067</v>
+      </c>
+      <c r="G126" t="n">
+        <v>912</v>
+      </c>
+      <c r="H126" t="s">
+        <v>176</v>
+      </c>
+      <c r="I126" t="s">
         <v>289</v>
-      </c>
-      <c r="D126" t="n">
-        <v>1305</v>
-      </c>
-      <c r="E126" t="n">
-        <v>1263</v>
-      </c>
-      <c r="F126" t="n">
-        <v>1024</v>
-      </c>
-      <c r="G126" t="n">
-        <v>991</v>
-      </c>
-      <c r="H126" t="s">
-        <v>59</v>
-      </c>
-      <c r="I126" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B127" t="n">
-        <v>136</v>
+        <v>2231</v>
       </c>
       <c r="C127" t="n">
-        <v>134</v>
+        <v>2159</v>
       </c>
       <c r="D127" t="n">
-        <v>694</v>
+        <v>9296</v>
       </c>
       <c r="E127" t="n">
-        <v>627</v>
+        <v>9164</v>
       </c>
       <c r="F127" t="n">
-        <v>484</v>
+        <v>7686</v>
       </c>
       <c r="G127" t="n">
-        <v>374</v>
+        <v>7420</v>
       </c>
       <c r="H127" t="s">
-        <v>273</v>
+        <v>95</v>
       </c>
       <c r="I127" t="s">
-        <v>288</v>
+        <v>56</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
+        <v>291</v>
+      </c>
+      <c r="B128" t="n">
+        <v>73</v>
+      </c>
+      <c r="C128" t="n">
+        <v>63</v>
+      </c>
+      <c r="D128" t="n">
+        <v>232</v>
+      </c>
+      <c r="E128" t="n">
+        <v>217</v>
+      </c>
+      <c r="F128" t="n">
+        <v>172</v>
+      </c>
+      <c r="G128" t="n">
+        <v>166</v>
+      </c>
+      <c r="H128" t="s">
+        <v>292</v>
+      </c>
+      <c r="I128" t="s">
         <v>289</v>
-      </c>
-      <c r="B128" t="n">
-        <v>253</v>
-      </c>
-      <c r="C128" t="n">
-        <v>263</v>
-      </c>
-      <c r="D128" t="n">
-        <v>1327</v>
-      </c>
-      <c r="E128" t="n">
-        <v>1192</v>
-      </c>
-      <c r="F128" t="n">
-        <v>1067</v>
-      </c>
-      <c r="G128" t="n">
-        <v>912</v>
-      </c>
-      <c r="H128" t="s">
-        <v>175</v>
-      </c>
-      <c r="I128" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B129" t="n">
-        <v>2231</v>
+        <v>70</v>
       </c>
       <c r="C129" t="n">
-        <v>2159</v>
+        <v>55</v>
       </c>
       <c r="D129" t="n">
-        <v>9296</v>
+        <v>241</v>
       </c>
       <c r="E129" t="n">
-        <v>9164</v>
+        <v>163</v>
       </c>
       <c r="F129" t="n">
-        <v>7686</v>
+        <v>204</v>
       </c>
       <c r="G129" t="n">
-        <v>7420</v>
+        <v>128</v>
       </c>
       <c r="H129" t="s">
-        <v>95</v>
+        <v>227</v>
       </c>
       <c r="I129" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B130" t="n">
-        <v>73</v>
+        <v>158</v>
       </c>
       <c r="C130" t="n">
-        <v>63</v>
+        <v>163</v>
       </c>
       <c r="D130" t="n">
-        <v>232</v>
+        <v>639</v>
       </c>
       <c r="E130" t="n">
-        <v>217</v>
+        <v>637</v>
       </c>
       <c r="F130" t="n">
-        <v>172</v>
+        <v>509</v>
       </c>
       <c r="G130" t="n">
-        <v>166</v>
+        <v>487</v>
       </c>
       <c r="H130" t="s">
-        <v>293</v>
+        <v>98</v>
       </c>
       <c r="I130" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B131" t="n">
-        <v>70</v>
+        <v>251</v>
       </c>
       <c r="C131" t="n">
-        <v>55</v>
+        <v>234</v>
       </c>
       <c r="D131" t="n">
-        <v>241</v>
+        <v>892</v>
       </c>
       <c r="E131" t="n">
-        <v>163</v>
+        <v>786</v>
       </c>
       <c r="F131" t="n">
-        <v>204</v>
+        <v>696</v>
       </c>
       <c r="G131" t="n">
-        <v>128</v>
+        <v>588</v>
       </c>
       <c r="H131" t="s">
-        <v>226</v>
+        <v>129</v>
       </c>
       <c r="I131" t="s">
-        <v>59</v>
+        <v>130</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B132" t="n">
-        <v>158</v>
+        <v>67</v>
       </c>
       <c r="C132" t="n">
-        <v>163</v>
+        <v>65</v>
       </c>
       <c r="D132" t="n">
-        <v>639</v>
+        <v>315</v>
       </c>
       <c r="E132" t="n">
-        <v>637</v>
+        <v>316</v>
       </c>
       <c r="F132" t="n">
-        <v>509</v>
+        <v>246</v>
       </c>
       <c r="G132" t="n">
-        <v>487</v>
+        <v>262</v>
       </c>
       <c r="H132" t="s">
-        <v>98</v>
+        <v>297</v>
       </c>
       <c r="I132" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B133" t="n">
-        <v>251</v>
+        <v>104</v>
       </c>
       <c r="C133" t="n">
-        <v>234</v>
+        <v>99</v>
       </c>
       <c r="D133" t="n">
-        <v>892</v>
+        <v>421</v>
       </c>
       <c r="E133" t="n">
-        <v>786</v>
+        <v>410</v>
       </c>
       <c r="F133" t="n">
-        <v>696</v>
+        <v>332</v>
       </c>
       <c r="G133" t="n">
-        <v>588</v>
+        <v>318</v>
       </c>
       <c r="H133" t="s">
-        <v>128</v>
+        <v>300</v>
       </c>
       <c r="I133" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B134" t="n">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="C134" t="n">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D134" t="n">
-        <v>315</v>
+        <v>371</v>
       </c>
       <c r="E134" t="n">
-        <v>316</v>
+        <v>478</v>
       </c>
       <c r="F134" t="n">
-        <v>246</v>
+        <v>276</v>
       </c>
       <c r="G134" t="n">
-        <v>262</v>
+        <v>328</v>
       </c>
       <c r="H134" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="I134" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B135" t="n">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="C135" t="n">
-        <v>99</v>
+        <v>132</v>
       </c>
       <c r="D135" t="n">
-        <v>421</v>
+        <v>466</v>
       </c>
       <c r="E135" t="n">
-        <v>410</v>
+        <v>595</v>
       </c>
       <c r="F135" t="n">
-        <v>332</v>
+        <v>386</v>
       </c>
       <c r="G135" t="n">
-        <v>318</v>
+        <v>501</v>
       </c>
       <c r="H135" t="s">
-        <v>301</v>
+        <v>239</v>
       </c>
       <c r="I135" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B136" t="n">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="C136" t="n">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D136" t="n">
-        <v>371</v>
+        <v>331</v>
       </c>
       <c r="E136" t="n">
-        <v>478</v>
+        <v>278</v>
       </c>
       <c r="F136" t="n">
-        <v>276</v>
+        <v>307</v>
       </c>
       <c r="G136" t="n">
-        <v>328</v>
+        <v>242</v>
       </c>
       <c r="H136" t="s">
-        <v>281</v>
+        <v>80</v>
       </c>
       <c r="I136" t="s">
-        <v>303</v>
+        <v>73</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B137" t="n">
-        <v>116</v>
+        <v>61</v>
       </c>
       <c r="C137" t="n">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="D137" t="n">
-        <v>466</v>
+        <v>210</v>
       </c>
       <c r="E137" t="n">
-        <v>595</v>
+        <v>171</v>
       </c>
       <c r="F137" t="n">
-        <v>386</v>
+        <v>161</v>
       </c>
       <c r="G137" t="n">
-        <v>501</v>
+        <v>145</v>
       </c>
       <c r="H137" t="s">
-        <v>239</v>
+        <v>306</v>
       </c>
       <c r="I137" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B138" t="n">
-        <v>75</v>
+        <v>212</v>
       </c>
       <c r="C138" t="n">
-        <v>67</v>
+        <v>232</v>
       </c>
       <c r="D138" t="n">
-        <v>331</v>
+        <v>971</v>
       </c>
       <c r="E138" t="n">
-        <v>278</v>
+        <v>1083</v>
       </c>
       <c r="F138" t="n">
-        <v>307</v>
+        <v>801</v>
       </c>
       <c r="G138" t="n">
-        <v>242</v>
+        <v>921</v>
       </c>
       <c r="H138" t="s">
-        <v>80</v>
+        <v>308</v>
       </c>
       <c r="I138" t="s">
-        <v>73</v>
+        <v>309</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B139" t="n">
-        <v>61</v>
+        <v>331</v>
       </c>
       <c r="C139" t="n">
-        <v>52</v>
+        <v>321</v>
       </c>
       <c r="D139" t="n">
-        <v>210</v>
+        <v>1371</v>
       </c>
       <c r="E139" t="n">
-        <v>171</v>
+        <v>1279</v>
       </c>
       <c r="F139" t="n">
-        <v>161</v>
+        <v>1127</v>
       </c>
       <c r="G139" t="n">
-        <v>145</v>
+        <v>1039</v>
       </c>
       <c r="H139" t="s">
-        <v>307</v>
+        <v>82</v>
       </c>
       <c r="I139" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B140" t="n">
-        <v>212</v>
+        <v>305</v>
       </c>
       <c r="C140" t="n">
-        <v>232</v>
+        <v>297</v>
       </c>
       <c r="D140" t="n">
-        <v>971</v>
+        <v>1490</v>
       </c>
       <c r="E140" t="n">
-        <v>1083</v>
+        <v>1413</v>
       </c>
       <c r="F140" t="n">
-        <v>801</v>
+        <v>1324</v>
       </c>
       <c r="G140" t="n">
-        <v>921</v>
+        <v>1187</v>
       </c>
       <c r="H140" t="s">
-        <v>309</v>
+        <v>68</v>
       </c>
       <c r="I140" t="s">
-        <v>310</v>
+        <v>91</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B141" t="n">
-        <v>331</v>
+        <v>310</v>
       </c>
       <c r="C141" t="n">
-        <v>321</v>
+        <v>298</v>
       </c>
       <c r="D141" t="n">
-        <v>1371</v>
+        <v>1346</v>
       </c>
       <c r="E141" t="n">
-        <v>1279</v>
+        <v>1338</v>
       </c>
       <c r="F141" t="n">
-        <v>1127</v>
+        <v>1145</v>
       </c>
       <c r="G141" t="n">
-        <v>1039</v>
+        <v>1108</v>
       </c>
       <c r="H141" t="s">
-        <v>82</v>
+        <v>313</v>
       </c>
       <c r="I141" t="s">
-        <v>83</v>
+        <v>239</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B142" t="n">
-        <v>305</v>
+        <v>2525</v>
       </c>
       <c r="C142" t="n">
-        <v>297</v>
+        <v>2495</v>
       </c>
       <c r="D142" t="n">
-        <v>1490</v>
+        <v>11536</v>
       </c>
       <c r="E142" t="n">
-        <v>1413</v>
+        <v>10822</v>
       </c>
       <c r="F142" t="n">
-        <v>1324</v>
+        <v>9508</v>
       </c>
       <c r="G142" t="n">
-        <v>1187</v>
+        <v>9184</v>
       </c>
       <c r="H142" t="s">
-        <v>68</v>
+        <v>315</v>
       </c>
       <c r="I142" t="s">
-        <v>91</v>
+        <v>316</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B143" t="n">
-        <v>310</v>
+        <v>217</v>
       </c>
       <c r="C143" t="n">
-        <v>298</v>
+        <v>215</v>
       </c>
       <c r="D143" t="n">
-        <v>1346</v>
+        <v>891</v>
       </c>
       <c r="E143" t="n">
-        <v>1338</v>
+        <v>918</v>
       </c>
       <c r="F143" t="n">
-        <v>1145</v>
+        <v>715</v>
       </c>
       <c r="G143" t="n">
-        <v>1108</v>
+        <v>771</v>
       </c>
       <c r="H143" t="s">
-        <v>314</v>
+        <v>178</v>
       </c>
       <c r="I143" t="s">
-        <v>239</v>
+        <v>91</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B144" t="n">
-        <v>2525</v>
+        <v>49</v>
       </c>
       <c r="C144" t="n">
-        <v>2495</v>
+        <v>48</v>
       </c>
       <c r="D144" t="n">
-        <v>11536</v>
+        <v>215</v>
       </c>
       <c r="E144" t="n">
-        <v>10822</v>
+        <v>199</v>
       </c>
       <c r="F144" t="n">
-        <v>9508</v>
+        <v>170</v>
       </c>
       <c r="G144" t="n">
-        <v>9184</v>
+        <v>159</v>
       </c>
       <c r="H144" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="I144" t="s">
-        <v>317</v>
+        <v>191</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B145" t="n">
-        <v>217</v>
+        <v>79</v>
       </c>
       <c r="C145" t="n">
-        <v>215</v>
+        <v>84</v>
       </c>
       <c r="D145" t="n">
-        <v>891</v>
+        <v>385</v>
       </c>
       <c r="E145" t="n">
-        <v>918</v>
+        <v>398</v>
       </c>
       <c r="F145" t="n">
-        <v>715</v>
+        <v>301</v>
       </c>
       <c r="G145" t="n">
-        <v>771</v>
+        <v>323</v>
       </c>
       <c r="H145" t="s">
-        <v>177</v>
+        <v>40</v>
       </c>
       <c r="I145" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B146" t="n">
+        <v>46</v>
+      </c>
+      <c r="C146" t="n">
         <v>49</v>
       </c>
-      <c r="C146" t="n">
-        <v>48</v>
-      </c>
       <c r="D146" t="n">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E146" t="n">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="F146" t="n">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G146" t="n">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H146" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="I146" t="s">
-        <v>190</v>
+        <v>263</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B147" t="n">
-        <v>79</v>
+        <v>130</v>
       </c>
       <c r="C147" t="n">
-        <v>84</v>
+        <v>128</v>
       </c>
       <c r="D147" t="n">
-        <v>385</v>
+        <v>654</v>
       </c>
       <c r="E147" t="n">
-        <v>398</v>
+        <v>617</v>
       </c>
       <c r="F147" t="n">
-        <v>301</v>
+        <v>551</v>
       </c>
       <c r="G147" t="n">
-        <v>323</v>
+        <v>537</v>
       </c>
       <c r="H147" t="s">
-        <v>40</v>
+        <v>252</v>
       </c>
       <c r="I147" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B148" t="n">
-        <v>46</v>
+        <v>173</v>
       </c>
       <c r="C148" t="n">
-        <v>49</v>
+        <v>174</v>
       </c>
       <c r="D148" t="n">
-        <v>211</v>
+        <v>647</v>
       </c>
       <c r="E148" t="n">
-        <v>206</v>
+        <v>656</v>
       </c>
       <c r="F148" t="n">
-        <v>168</v>
+        <v>533</v>
       </c>
       <c r="G148" t="n">
-        <v>153</v>
+        <v>582</v>
       </c>
       <c r="H148" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="I148" t="s">
-        <v>264</v>
+        <v>69</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B149" t="n">
-        <v>130</v>
+        <v>224</v>
       </c>
       <c r="C149" t="n">
-        <v>128</v>
+        <v>231</v>
       </c>
       <c r="D149" t="n">
-        <v>654</v>
+        <v>1128</v>
       </c>
       <c r="E149" t="n">
-        <v>617</v>
+        <v>1085</v>
       </c>
       <c r="F149" t="n">
-        <v>551</v>
+        <v>961</v>
       </c>
       <c r="G149" t="n">
-        <v>537</v>
+        <v>952</v>
       </c>
       <c r="H149" t="s">
-        <v>253</v>
+        <v>20</v>
       </c>
       <c r="I149" t="s">
-        <v>85</v>
+        <v>230</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B150" t="n">
-        <v>173</v>
+        <v>105</v>
       </c>
       <c r="C150" t="n">
-        <v>174</v>
+        <v>91</v>
       </c>
       <c r="D150" t="n">
-        <v>647</v>
+        <v>457</v>
       </c>
       <c r="E150" t="n">
-        <v>656</v>
+        <v>427</v>
       </c>
       <c r="F150" t="n">
-        <v>533</v>
+        <v>343</v>
       </c>
       <c r="G150" t="n">
-        <v>582</v>
+        <v>338</v>
       </c>
       <c r="H150" t="s">
-        <v>316</v>
+        <v>276</v>
       </c>
       <c r="I150" t="s">
-        <v>69</v>
+        <v>171</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B151" t="n">
-        <v>224</v>
+        <v>184</v>
       </c>
       <c r="C151" t="n">
-        <v>231</v>
+        <v>190</v>
       </c>
       <c r="D151" t="n">
-        <v>1128</v>
+        <v>967</v>
       </c>
       <c r="E151" t="n">
-        <v>1085</v>
+        <v>895</v>
       </c>
       <c r="F151" t="n">
-        <v>961</v>
+        <v>827</v>
       </c>
       <c r="G151" t="n">
-        <v>952</v>
+        <v>811</v>
       </c>
       <c r="H151" t="s">
-        <v>20</v>
+        <v>328</v>
       </c>
       <c r="I151" t="s">
-        <v>229</v>
+        <v>154</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B152" t="n">
-        <v>105</v>
+        <v>370</v>
       </c>
       <c r="C152" t="n">
-        <v>91</v>
+        <v>368</v>
       </c>
       <c r="D152" t="n">
-        <v>457</v>
+        <v>1613</v>
       </c>
       <c r="E152" t="n">
-        <v>427</v>
+        <v>1521</v>
       </c>
       <c r="F152" t="n">
-        <v>343</v>
+        <v>1278</v>
       </c>
       <c r="G152" t="n">
-        <v>338</v>
+        <v>1267</v>
       </c>
       <c r="H152" t="s">
-        <v>277</v>
+        <v>171</v>
       </c>
       <c r="I152" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B153" t="n">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="C153" t="n">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D153" t="n">
-        <v>967</v>
+        <v>862</v>
       </c>
       <c r="E153" t="n">
-        <v>895</v>
+        <v>860</v>
       </c>
       <c r="F153" t="n">
-        <v>827</v>
+        <v>723</v>
       </c>
       <c r="G153" t="n">
-        <v>811</v>
+        <v>738</v>
       </c>
       <c r="H153" t="s">
-        <v>329</v>
+        <v>202</v>
       </c>
       <c r="I153" t="s">
-        <v>153</v>
+        <v>331</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B154" t="n">
-        <v>370</v>
+        <v>162</v>
       </c>
       <c r="C154" t="n">
-        <v>368</v>
+        <v>168</v>
       </c>
       <c r="D154" t="n">
-        <v>1613</v>
+        <v>673</v>
       </c>
       <c r="E154" t="n">
-        <v>1521</v>
+        <v>712</v>
       </c>
       <c r="F154" t="n">
-        <v>1278</v>
+        <v>510</v>
       </c>
       <c r="G154" t="n">
-        <v>1267</v>
+        <v>584</v>
       </c>
       <c r="H154" t="s">
-        <v>170</v>
+        <v>333</v>
       </c>
       <c r="I154" t="s">
-        <v>198</v>
+        <v>334</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B155" t="n">
-        <v>195</v>
+        <v>103</v>
       </c>
       <c r="C155" t="n">
-        <v>194</v>
+        <v>99</v>
       </c>
       <c r="D155" t="n">
-        <v>862</v>
+        <v>479</v>
       </c>
       <c r="E155" t="n">
-        <v>860</v>
+        <v>403</v>
       </c>
       <c r="F155" t="n">
-        <v>723</v>
+        <v>390</v>
       </c>
       <c r="G155" t="n">
-        <v>738</v>
+        <v>318</v>
       </c>
       <c r="H155" t="s">
-        <v>201</v>
+        <v>240</v>
       </c>
       <c r="I155" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B156" t="n">
-        <v>162</v>
+        <v>195</v>
       </c>
       <c r="C156" t="n">
-        <v>168</v>
+        <v>200</v>
       </c>
       <c r="D156" t="n">
-        <v>673</v>
+        <v>915</v>
       </c>
       <c r="E156" t="n">
-        <v>712</v>
+        <v>796</v>
       </c>
       <c r="F156" t="n">
-        <v>510</v>
+        <v>773</v>
       </c>
       <c r="G156" t="n">
-        <v>584</v>
+        <v>664</v>
       </c>
       <c r="H156" t="s">
-        <v>334</v>
+        <v>211</v>
       </c>
       <c r="I156" t="s">
-        <v>335</v>
+        <v>37</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B157" t="n">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="C157" t="n">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D157" t="n">
-        <v>479</v>
+        <v>638</v>
       </c>
       <c r="E157" t="n">
-        <v>403</v>
+        <v>432</v>
       </c>
       <c r="F157" t="n">
-        <v>390</v>
+        <v>564</v>
       </c>
       <c r="G157" t="n">
-        <v>318</v>
+        <v>396</v>
       </c>
       <c r="H157" t="s">
-        <v>240</v>
+        <v>338</v>
       </c>
       <c r="I157" t="s">
-        <v>301</v>
+        <v>77</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B158" t="n">
-        <v>195</v>
+        <v>26</v>
       </c>
       <c r="C158" t="n">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="D158" t="n">
-        <v>915</v>
+        <v>127</v>
       </c>
       <c r="E158" t="n">
-        <v>796</v>
+        <v>34</v>
       </c>
       <c r="F158" t="n">
-        <v>773</v>
+        <v>127</v>
       </c>
       <c r="G158" t="n">
-        <v>664</v>
+        <v>34</v>
       </c>
       <c r="H158" t="s">
-        <v>210</v>
+        <v>119</v>
       </c>
       <c r="I158" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B159" t="n">
-        <v>125</v>
+        <v>43</v>
       </c>
       <c r="C159" t="n">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="D159" t="n">
-        <v>638</v>
+        <v>168</v>
       </c>
       <c r="E159" t="n">
-        <v>432</v>
+        <v>183</v>
       </c>
       <c r="F159" t="n">
-        <v>564</v>
+        <v>120</v>
       </c>
       <c r="G159" t="n">
-        <v>396</v>
+        <v>158</v>
       </c>
       <c r="H159" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="I159" t="s">
-        <v>77</v>
+        <v>342</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B160" t="n">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C160" t="n">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="D160" t="n">
-        <v>127</v>
+        <v>230</v>
       </c>
       <c r="E160" t="n">
-        <v>34</v>
+        <v>224</v>
       </c>
       <c r="F160" t="n">
-        <v>127</v>
+        <v>206</v>
       </c>
       <c r="G160" t="n">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="H160" t="s">
-        <v>119</v>
+        <v>344</v>
       </c>
       <c r="I160" t="s">
-        <v>119</v>
+        <v>202</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="B161" t="n">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C161" t="n">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D161" t="n">
-        <v>168</v>
+        <v>276</v>
       </c>
       <c r="E161" t="n">
-        <v>183</v>
+        <v>256</v>
       </c>
       <c r="F161" t="n">
-        <v>120</v>
+        <v>248</v>
       </c>
       <c r="G161" t="n">
-        <v>158</v>
+        <v>211</v>
       </c>
       <c r="H161" t="s">
-        <v>342</v>
+        <v>86</v>
       </c>
       <c r="I161" t="s">
-        <v>343</v>
+        <v>315</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B162" t="n">
-        <v>42</v>
+        <v>659</v>
       </c>
       <c r="C162" t="n">
-        <v>42</v>
+        <v>578</v>
       </c>
       <c r="D162" t="n">
-        <v>230</v>
+        <v>3185</v>
       </c>
       <c r="E162" t="n">
-        <v>224</v>
+        <v>2660</v>
       </c>
       <c r="F162" t="n">
-        <v>206</v>
+        <v>2891</v>
       </c>
       <c r="G162" t="n">
-        <v>188</v>
+        <v>2451</v>
       </c>
       <c r="H162" t="s">
-        <v>345</v>
+        <v>66</v>
       </c>
       <c r="I162" t="s">
-        <v>201</v>
+        <v>30</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B163" t="n">
-        <v>57</v>
+        <v>460</v>
       </c>
       <c r="C163" t="n">
-        <v>56</v>
+        <v>430</v>
       </c>
       <c r="D163" t="n">
-        <v>276</v>
+        <v>2296</v>
       </c>
       <c r="E163" t="n">
-        <v>256</v>
+        <v>1986</v>
       </c>
       <c r="F163" t="n">
-        <v>248</v>
+        <v>2088</v>
       </c>
       <c r="G163" t="n">
-        <v>211</v>
+        <v>1831</v>
       </c>
       <c r="H163" t="s">
-        <v>86</v>
+        <v>348</v>
       </c>
       <c r="I163" t="s">
-        <v>316</v>
+        <v>349</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="B164" t="n">
-        <v>659</v>
+        <v>93</v>
       </c>
       <c r="C164" t="n">
-        <v>578</v>
+        <v>91</v>
       </c>
       <c r="D164" t="n">
-        <v>3185</v>
+        <v>471</v>
       </c>
       <c r="E164" t="n">
-        <v>2660</v>
+        <v>497</v>
       </c>
       <c r="F164" t="n">
-        <v>2891</v>
+        <v>436</v>
       </c>
       <c r="G164" t="n">
-        <v>2451</v>
+        <v>466</v>
       </c>
       <c r="H164" t="s">
-        <v>66</v>
+        <v>351</v>
       </c>
       <c r="I164" t="s">
-        <v>30</v>
+        <v>352</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="B165" t="n">
-        <v>460</v>
+        <v>68</v>
       </c>
       <c r="C165" t="n">
-        <v>430</v>
+        <v>29</v>
       </c>
       <c r="D165" t="n">
-        <v>2296</v>
+        <v>282</v>
       </c>
       <c r="E165" t="n">
-        <v>1986</v>
+        <v>101</v>
       </c>
       <c r="F165" t="n">
-        <v>2088</v>
+        <v>257</v>
       </c>
       <c r="G165" t="n">
-        <v>1831</v>
+        <v>92</v>
       </c>
       <c r="H165" t="s">
-        <v>349</v>
+        <v>65</v>
       </c>
       <c r="I165" t="s">
-        <v>350</v>
+        <v>65</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B166" t="n">
-        <v>93</v>
+        <v>38</v>
       </c>
       <c r="C166" t="n">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="D166" t="n">
-        <v>471</v>
+        <v>136</v>
       </c>
       <c r="E166" t="n">
-        <v>497</v>
+        <v>76</v>
       </c>
       <c r="F166" t="n">
-        <v>436</v>
+        <v>110</v>
       </c>
       <c r="G166" t="n">
-        <v>466</v>
+        <v>62</v>
       </c>
       <c r="H166" t="s">
-        <v>352</v>
+        <v>43</v>
       </c>
       <c r="I166" t="s">
-        <v>353</v>
+        <v>204</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B167" t="n">
-        <v>68</v>
+        <v>401</v>
       </c>
       <c r="C167" t="n">
-        <v>29</v>
+        <v>394</v>
       </c>
       <c r="D167" t="n">
-        <v>282</v>
+        <v>2094</v>
       </c>
       <c r="E167" t="n">
-        <v>101</v>
+        <v>1948</v>
       </c>
       <c r="F167" t="n">
-        <v>257</v>
+        <v>1770</v>
       </c>
       <c r="G167" t="n">
-        <v>92</v>
+        <v>1645</v>
       </c>
       <c r="H167" t="s">
-        <v>65</v>
+        <v>211</v>
       </c>
       <c r="I167" t="s">
-        <v>65</v>
+        <v>225</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B168" t="n">
-        <v>38</v>
+        <v>401</v>
       </c>
       <c r="C168" t="n">
-        <v>28</v>
+        <v>394</v>
       </c>
       <c r="D168" t="n">
-        <v>136</v>
+        <v>2094</v>
       </c>
       <c r="E168" t="n">
-        <v>76</v>
+        <v>1948</v>
       </c>
       <c r="F168" t="n">
-        <v>110</v>
+        <v>1770</v>
       </c>
       <c r="G168" t="n">
-        <v>62</v>
+        <v>1645</v>
       </c>
       <c r="H168" t="s">
-        <v>43</v>
+        <v>211</v>
       </c>
       <c r="I168" t="s">
-        <v>203</v>
+        <v>225</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B169" t="n">
-        <v>401</v>
+        <v>950</v>
       </c>
       <c r="C169" t="n">
-        <v>394</v>
+        <v>901</v>
       </c>
       <c r="D169" t="n">
-        <v>2094</v>
+        <v>5525</v>
       </c>
       <c r="E169" t="n">
-        <v>1948</v>
+        <v>5126</v>
       </c>
       <c r="F169" t="n">
-        <v>1770</v>
+        <v>4292</v>
       </c>
       <c r="G169" t="n">
-        <v>1645</v>
+        <v>3987</v>
       </c>
       <c r="H169" t="s">
-        <v>210</v>
+        <v>250</v>
       </c>
       <c r="I169" t="s">
-        <v>224</v>
+        <v>139</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B170" t="n">
-        <v>401</v>
+        <v>337</v>
       </c>
       <c r="C170" t="n">
-        <v>394</v>
+        <v>323</v>
       </c>
       <c r="D170" t="n">
-        <v>2094</v>
+        <v>2180</v>
       </c>
       <c r="E170" t="n">
-        <v>1948</v>
+        <v>1919</v>
       </c>
       <c r="F170" t="n">
-        <v>1770</v>
+        <v>1857</v>
       </c>
       <c r="G170" t="n">
-        <v>1645</v>
+        <v>1586</v>
       </c>
       <c r="H170" t="s">
-        <v>210</v>
+        <v>20</v>
       </c>
       <c r="I170" t="s">
-        <v>224</v>
+        <v>26</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B171" t="n">
-        <v>950</v>
+        <v>195</v>
       </c>
       <c r="C171" t="n">
-        <v>901</v>
+        <v>185</v>
       </c>
       <c r="D171" t="n">
-        <v>5525</v>
+        <v>1084</v>
       </c>
       <c r="E171" t="n">
-        <v>5126</v>
+        <v>1108</v>
       </c>
       <c r="F171" t="n">
-        <v>4292</v>
+        <v>823</v>
       </c>
       <c r="G171" t="n">
-        <v>3987</v>
+        <v>842</v>
       </c>
       <c r="H171" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="I171" t="s">
-        <v>138</v>
+        <v>63</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B172" t="n">
-        <v>337</v>
+        <v>210</v>
       </c>
       <c r="C172" t="n">
-        <v>323</v>
+        <v>210</v>
       </c>
       <c r="D172" t="n">
-        <v>2180</v>
+        <v>1177</v>
       </c>
       <c r="E172" t="n">
-        <v>1919</v>
+        <v>1095</v>
       </c>
       <c r="F172" t="n">
-        <v>1857</v>
+        <v>844</v>
       </c>
       <c r="G172" t="n">
-        <v>1586</v>
+        <v>795</v>
       </c>
       <c r="H172" t="s">
-        <v>20</v>
+        <v>361</v>
       </c>
       <c r="I172" t="s">
-        <v>26</v>
+        <v>362</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B173" t="n">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="C173" t="n">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D173" t="n">
         <v>1084</v>
       </c>
       <c r="E173" t="n">
-        <v>1108</v>
+        <v>1004</v>
       </c>
       <c r="F173" t="n">
-        <v>823</v>
+        <v>768</v>
       </c>
       <c r="G173" t="n">
-        <v>842</v>
+        <v>764</v>
       </c>
       <c r="H173" t="s">
-        <v>257</v>
+        <v>364</v>
       </c>
       <c r="I173" t="s">
-        <v>63</v>
+        <v>173</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="B174" t="n">
-        <v>210</v>
+        <v>435</v>
       </c>
       <c r="C174" t="n">
-        <v>210</v>
+        <v>447</v>
       </c>
       <c r="D174" t="n">
-        <v>1177</v>
+        <v>2295</v>
       </c>
       <c r="E174" t="n">
-        <v>1095</v>
+        <v>2126</v>
       </c>
       <c r="F174" t="n">
-        <v>844</v>
+        <v>2095</v>
       </c>
       <c r="G174" t="n">
-        <v>795</v>
+        <v>1933</v>
       </c>
       <c r="H174" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="I174" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="B175" t="n">
-        <v>208</v>
+        <v>435</v>
       </c>
       <c r="C175" t="n">
-        <v>183</v>
+        <v>447</v>
       </c>
       <c r="D175" t="n">
-        <v>1084</v>
+        <v>2295</v>
       </c>
       <c r="E175" t="n">
-        <v>1004</v>
+        <v>2126</v>
       </c>
       <c r="F175" t="n">
-        <v>768</v>
+        <v>2095</v>
       </c>
       <c r="G175" t="n">
-        <v>764</v>
+        <v>1933</v>
       </c>
       <c r="H175" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="I175" t="s">
-        <v>172</v>
+        <v>348</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B176" t="n">
-        <v>435</v>
+        <v>34138</v>
       </c>
       <c r="C176" t="n">
-        <v>447</v>
+        <v>33626</v>
       </c>
       <c r="D176" t="n">
-        <v>2295</v>
+        <v>177845</v>
       </c>
       <c r="E176" t="n">
-        <v>2126</v>
+        <v>167485</v>
       </c>
       <c r="F176" t="n">
-        <v>2095</v>
+        <v>147696</v>
       </c>
       <c r="G176" t="n">
-        <v>1933</v>
+        <v>139235</v>
       </c>
       <c r="H176" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="I176" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="s">
-        <v>368</v>
-      </c>
-      <c r="B177" t="n">
-        <v>435</v>
-      </c>
-      <c r="C177" t="n">
-        <v>447</v>
-      </c>
-      <c r="D177" t="n">
-        <v>2295</v>
-      </c>
-      <c r="E177" t="n">
-        <v>2126</v>
-      </c>
-      <c r="F177" t="n">
-        <v>2095</v>
-      </c>
-      <c r="G177" t="n">
-        <v>1933</v>
-      </c>
-      <c r="H177" t="s">
-        <v>367</v>
-      </c>
-      <c r="I177" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="s">
-        <v>369</v>
-      </c>
-      <c r="B178" t="n">
-        <v>34138</v>
-      </c>
-      <c r="C178" t="n">
-        <v>33626</v>
-      </c>
-      <c r="D178" t="n">
-        <v>177845</v>
-      </c>
-      <c r="E178" t="n">
-        <v>167485</v>
-      </c>
-      <c r="F178" t="n">
-        <v>147696</v>
-      </c>
-      <c r="G178" t="n">
-        <v>139235</v>
-      </c>
-      <c r="H178" t="s">
-        <v>370</v>
-      </c>
-      <c r="I178" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>